<commit_message>
Changing GUI layout and adding notebook functionality (no rendering yet)
</commit_message>
<xml_diff>
--- a/Ortho_App/gui_data.xlsx
+++ b/Ortho_App/gui_data.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,6 +512,336 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 02:53:02 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 02:56:42 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 03:04:47 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 03:15:29 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 03:17:16 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thu 06 Feb 2025 07:58:59 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>New2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fri 07 Feb 2025 11:43:27 AM MST
+</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fri 07 Feb 2025 11:43:42 AM MST
+</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>New3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fri 07 Feb 2025 12:08:40 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fri 07 Feb 2025 12:12:28 PM MST
+</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>amatos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Lange</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>